<commit_message>
update journal Nelson Cuervo
</commit_message>
<xml_diff>
--- a/NelsonCuervo/Sprint3/Sprint3Planning.xlsx
+++ b/NelsonCuervo/Sprint3/Sprint3Planning.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson\Dropbox\PC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson\Dropbox\PC\Desktop\DEVELOPPEMENT-APPLICATIOS\projetChantier\NelsonCuervo\Sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45D2BC4F-E57E-45E0-8C3E-933A6BB2B199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B3151E-318C-4961-AD24-5B8F2BECDE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{49593094-89CE-44F8-8C8B-C49636785A2F}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Le cahier des charges" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sprint 1'!$B$27:$I$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sprint 1'!$B$27:$I$85</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -837,10 +837,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49990737-28A7-44F3-B503-5D019EA27ABA}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:XFD108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47:C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33786,7 +33787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:16384" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16384" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="13">
         <v>1</v>
       </c>
@@ -33808,7 +33809,7 @@
       <c r="L28" s="13"/>
       <c r="M28" s="13"/>
     </row>
-    <row r="29" spans="1:16384" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16384" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="19">
         <v>2</v>
       </c>
@@ -33836,7 +33837,7 @@
       <c r="L29" s="19"/>
       <c r="M29" s="19"/>
     </row>
-    <row r="30" spans="1:16384" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16384" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="13">
         <v>3</v>
       </c>
@@ -33892,7 +33893,7 @@
       <c r="L31" s="19"/>
       <c r="M31" s="19"/>
     </row>
-    <row r="32" spans="1:16384" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16384" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="13">
         <v>5</v>
       </c>
@@ -33918,7 +33919,7 @@
       <c r="L32" s="13"/>
       <c r="M32" s="13"/>
     </row>
-    <row r="33" spans="1:347" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="19">
         <v>6</v>
       </c>
@@ -33944,7 +33945,7 @@
       <c r="L33" s="19"/>
       <c r="M33" s="19"/>
     </row>
-    <row r="34" spans="1:347" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34" s="13">
         <v>7</v>
       </c>
@@ -33970,7 +33971,7 @@
       <c r="L34" s="13"/>
       <c r="M34" s="13"/>
     </row>
-    <row r="35" spans="1:347" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="19">
         <v>8</v>
       </c>
@@ -33996,7 +33997,7 @@
       <c r="L35" s="19"/>
       <c r="M35" s="19"/>
     </row>
-    <row r="36" spans="1:347" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="13">
         <v>9</v>
       </c>
@@ -34022,7 +34023,7 @@
       <c r="L36" s="13"/>
       <c r="M36" s="13"/>
     </row>
-    <row r="37" spans="1:347" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="19">
         <v>10</v>
       </c>
@@ -34074,7 +34075,7 @@
       <c r="L38" s="13"/>
       <c r="M38" s="13"/>
     </row>
-    <row r="39" spans="1:347" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>12</v>
       </c>
@@ -34097,7 +34098,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:347" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:347" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40" s="2">
         <v>13</v>
@@ -34455,7 +34456,7 @@
       <c r="MH40"/>
       <c r="MI40"/>
     </row>
-    <row r="41" spans="1:347" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>14</v>
       </c>
@@ -34836,7 +34837,7 @@
       <c r="MH42"/>
       <c r="MI42"/>
     </row>
-    <row r="43" spans="1:347" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:347" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43"/>
       <c r="B43">
         <v>16</v>
@@ -34865,7 +34866,7 @@
       <c r="L43"/>
       <c r="M43"/>
     </row>
-    <row r="44" spans="1:347" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:347" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44"/>
       <c r="B44" s="2">
         <v>17</v>
@@ -35228,7 +35229,7 @@
       <c r="MH44" s="1"/>
       <c r="MI44" s="1"/>
     </row>
-    <row r="45" spans="1:347" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:347" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45"/>
       <c r="B45">
         <v>18</v>
@@ -35257,7 +35258,7 @@
       <c r="L45" s="27"/>
       <c r="M45" s="27"/>
     </row>
-    <row r="46" spans="1:347" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:347" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46"/>
       <c r="B46" s="2">
         <v>19</v>
@@ -38964,7 +38965,7 @@
       <c r="MH64"/>
       <c r="MI64"/>
     </row>
-    <row r="65" spans="1:347" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>38</v>
       </c>
@@ -38981,7 +38982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:347" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:347" s="34" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66"/>
       <c r="B66" s="34">
         <v>39</v>
@@ -39333,7 +39334,7 @@
       <c r="MH66"/>
       <c r="MI66"/>
     </row>
-    <row r="67" spans="1:347" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>40</v>
       </c>
@@ -39350,7 +39351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:347" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:347" s="34" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68"/>
       <c r="B68" s="34">
         <v>41</v>
@@ -39702,7 +39703,7 @@
       <c r="MH68"/>
       <c r="MI68"/>
     </row>
-    <row r="69" spans="1:347" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>42</v>
       </c>
@@ -39719,7 +39720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:347" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:347" s="34" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70"/>
       <c r="B70" s="34">
         <v>43</v>
@@ -40071,7 +40072,7 @@
       <c r="MH70"/>
       <c r="MI70"/>
     </row>
-    <row r="71" spans="1:347" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>44</v>
       </c>
@@ -40088,7 +40089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:347" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:347" s="34" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72"/>
       <c r="B72" s="34">
         <v>45</v>
@@ -42697,7 +42698,14 @@
       <c r="D108"/>
     </row>
   </sheetData>
-  <autoFilter ref="B27:I27" xr:uid="{49990737-28A7-44F3-B503-5D019EA27ABA}"/>
+  <autoFilter ref="B27:I85" xr:uid="{49990737-28A7-44F3-B503-5D019EA27ABA}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Leonel - Nelson"/>
+        <filter val="Nelson"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update SpringPlaning -- Nelson Cuervo folder
</commit_message>
<xml_diff>
--- a/NelsonCuervo/Sprint3/Sprint3Planning.xlsx
+++ b/NelsonCuervo/Sprint3/Sprint3Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelson\Dropbox\PC\Desktop\DEVELOPPEMENT-APPLICATIOS\projetChantier\NelsonCuervo\Sprint3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B3151E-318C-4961-AD24-5B8F2BECDE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D4ACD2-B4D6-4DFD-A7C0-FEAEC61914B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{49593094-89CE-44F8-8C8B-C49636785A2F}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="96">
   <si>
     <t>Sprint Goal:</t>
   </si>
@@ -315,6 +315,9 @@
   </si>
   <si>
     <t>Leonel - Nelson</t>
+  </si>
+  <si>
+    <t>Nelson - Leonel</t>
   </si>
 </sst>
 </file>
@@ -837,11 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49990737-28A7-44F3-B503-5D019EA27ABA}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:XFD108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47:C85"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33787,7 +33789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:16384" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16384" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="13">
         <v>1</v>
       </c>
@@ -33809,7 +33811,7 @@
       <c r="L28" s="13"/>
       <c r="M28" s="13"/>
     </row>
-    <row r="29" spans="1:16384" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16384" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="19">
         <v>2</v>
       </c>
@@ -33837,7 +33839,7 @@
       <c r="L29" s="19"/>
       <c r="M29" s="19"/>
     </row>
-    <row r="30" spans="1:16384" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16384" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="13">
         <v>3</v>
       </c>
@@ -33893,7 +33895,7 @@
       <c r="L31" s="19"/>
       <c r="M31" s="19"/>
     </row>
-    <row r="32" spans="1:16384" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16384" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="13">
         <v>5</v>
       </c>
@@ -33919,7 +33921,7 @@
       <c r="L32" s="13"/>
       <c r="M32" s="13"/>
     </row>
-    <row r="33" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:347" x14ac:dyDescent="0.25">
       <c r="B33" s="19">
         <v>6</v>
       </c>
@@ -33945,7 +33947,7 @@
       <c r="L33" s="19"/>
       <c r="M33" s="19"/>
     </row>
-    <row r="34" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:347" x14ac:dyDescent="0.25">
       <c r="B34" s="13">
         <v>7</v>
       </c>
@@ -33971,7 +33973,7 @@
       <c r="L34" s="13"/>
       <c r="M34" s="13"/>
     </row>
-    <row r="35" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:347" x14ac:dyDescent="0.25">
       <c r="B35" s="19">
         <v>8</v>
       </c>
@@ -33997,7 +33999,7 @@
       <c r="L35" s="19"/>
       <c r="M35" s="19"/>
     </row>
-    <row r="36" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:347" x14ac:dyDescent="0.25">
       <c r="B36" s="13">
         <v>9</v>
       </c>
@@ -34023,7 +34025,7 @@
       <c r="L36" s="13"/>
       <c r="M36" s="13"/>
     </row>
-    <row r="37" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:347" x14ac:dyDescent="0.25">
       <c r="B37" s="19">
         <v>10</v>
       </c>
@@ -34075,7 +34077,7 @@
       <c r="L38" s="13"/>
       <c r="M38" s="13"/>
     </row>
-    <row r="39" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:347" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>12</v>
       </c>
@@ -34098,7 +34100,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:347" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:347" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40" s="2">
         <v>13</v>
@@ -34456,7 +34458,7 @@
       <c r="MH40"/>
       <c r="MI40"/>
     </row>
-    <row r="41" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:347" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>14</v>
       </c>
@@ -34837,7 +34839,7 @@
       <c r="MH42"/>
       <c r="MI42"/>
     </row>
-    <row r="43" spans="1:347" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:347" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43"/>
       <c r="B43">
         <v>16</v>
@@ -34866,7 +34868,7 @@
       <c r="L43"/>
       <c r="M43"/>
     </row>
-    <row r="44" spans="1:347" s="22" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:347" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44"/>
       <c r="B44" s="2">
         <v>17</v>
@@ -35229,7 +35231,7 @@
       <c r="MH44" s="1"/>
       <c r="MI44" s="1"/>
     </row>
-    <row r="45" spans="1:347" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:347" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45"/>
       <c r="B45">
         <v>18</v>
@@ -35258,7 +35260,7 @@
       <c r="L45" s="27"/>
       <c r="M45" s="27"/>
     </row>
-    <row r="46" spans="1:347" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:347" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46"/>
       <c r="B46" s="2">
         <v>19</v>
@@ -35611,7 +35613,7 @@
         <v>3</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F47" s="1">
         <v>1</v>
@@ -35635,8 +35637,8 @@
       <c r="D48" s="32">
         <v>3</v>
       </c>
-      <c r="E48" s="31" t="s">
-        <v>49</v>
+      <c r="E48" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F48" s="1">
         <v>1</v>
@@ -35995,7 +35997,7 @@
         <v>3</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F49" s="1">
         <v>1</v>
@@ -36019,8 +36021,8 @@
       <c r="D50" s="32">
         <v>3</v>
       </c>
-      <c r="E50" s="31" t="s">
-        <v>49</v>
+      <c r="E50" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F50" s="1">
         <v>1</v>
@@ -36378,7 +36380,7 @@
         <v>3</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F51" s="1">
         <v>1</v>
@@ -36402,8 +36404,8 @@
       <c r="D52" s="32">
         <v>3</v>
       </c>
-      <c r="E52" s="31" t="s">
-        <v>49</v>
+      <c r="E52" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F52" s="1">
         <v>1</v>
@@ -36761,7 +36763,7 @@
         <v>3</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F53" s="1">
         <v>1</v>
@@ -36779,8 +36781,8 @@
       <c r="D54" s="32">
         <v>3</v>
       </c>
-      <c r="E54" s="31" t="s">
-        <v>49</v>
+      <c r="E54" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F54" s="1">
         <v>1</v>
@@ -37131,7 +37133,7 @@
         <v>3</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F55" s="1">
         <v>1</v>
@@ -37148,8 +37150,8 @@
       <c r="D56" s="32">
         <v>3</v>
       </c>
-      <c r="E56" s="31" t="s">
-        <v>49</v>
+      <c r="E56" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F56" s="1">
         <v>1</v>
@@ -37500,7 +37502,7 @@
         <v>3</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F57" s="1">
         <v>1</v>
@@ -37517,8 +37519,8 @@
       <c r="D58" s="32">
         <v>3</v>
       </c>
-      <c r="E58" s="31" t="s">
-        <v>49</v>
+      <c r="E58" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F58" s="1">
         <v>1</v>
@@ -37869,7 +37871,7 @@
         <v>3</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F59" s="1">
         <v>1</v>
@@ -37886,8 +37888,8 @@
       <c r="D60" s="32">
         <v>3</v>
       </c>
-      <c r="E60" s="31" t="s">
-        <v>49</v>
+      <c r="E60" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F60" s="1">
         <v>1</v>
@@ -38238,7 +38240,7 @@
         <v>3</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F61" s="1">
         <v>1</v>
@@ -38255,8 +38257,8 @@
       <c r="D62" s="32">
         <v>3</v>
       </c>
-      <c r="E62" s="31" t="s">
-        <v>49</v>
+      <c r="E62" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F62" s="1">
         <v>1</v>
@@ -38607,7 +38609,7 @@
         <v>3</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F63" s="1">
         <v>1</v>
@@ -38624,8 +38626,8 @@
       <c r="D64" s="32">
         <v>3</v>
       </c>
-      <c r="E64" s="31" t="s">
-        <v>49</v>
+      <c r="E64" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F64" s="1">
         <v>1</v>
@@ -38965,7 +38967,7 @@
       <c r="MH64"/>
       <c r="MI64"/>
     </row>
-    <row r="65" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:347" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>38</v>
       </c>
@@ -38976,13 +38978,13 @@
         <v>3</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="F65" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:347" s="34" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:347" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66"/>
       <c r="B66" s="34">
         <v>39</v>
@@ -38993,8 +38995,8 @@
       <c r="D66" s="32">
         <v>3</v>
       </c>
-      <c r="E66" s="31" t="s">
-        <v>55</v>
+      <c r="E66" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F66" s="1">
         <v>1</v>
@@ -39334,7 +39336,7 @@
       <c r="MH66"/>
       <c r="MI66"/>
     </row>
-    <row r="67" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:347" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>40</v>
       </c>
@@ -39345,13 +39347,13 @@
         <v>3</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="F67" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:347" s="34" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:347" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68"/>
       <c r="B68" s="34">
         <v>41</v>
@@ -39362,8 +39364,8 @@
       <c r="D68" s="32">
         <v>3</v>
       </c>
-      <c r="E68" s="31" t="s">
-        <v>55</v>
+      <c r="E68" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F68" s="1">
         <v>1</v>
@@ -39703,7 +39705,7 @@
       <c r="MH68"/>
       <c r="MI68"/>
     </row>
-    <row r="69" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:347" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>42</v>
       </c>
@@ -39714,13 +39716,13 @@
         <v>3</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="F69" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:347" s="34" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:347" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70"/>
       <c r="B70" s="34">
         <v>43</v>
@@ -39731,8 +39733,8 @@
       <c r="D70" s="32">
         <v>3</v>
       </c>
-      <c r="E70" s="31" t="s">
-        <v>55</v>
+      <c r="E70" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F70" s="1">
         <v>1</v>
@@ -40072,7 +40074,7 @@
       <c r="MH70"/>
       <c r="MI70"/>
     </row>
-    <row r="71" spans="1:347" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:347" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>44</v>
       </c>
@@ -40083,13 +40085,13 @@
         <v>3</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="F71" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:347" s="34" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:347" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72"/>
       <c r="B72" s="34">
         <v>45</v>
@@ -40100,8 +40102,8 @@
       <c r="D72" s="32">
         <v>3</v>
       </c>
-      <c r="E72" s="31" t="s">
-        <v>55</v>
+      <c r="E72" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F72" s="1">
         <v>1</v>
@@ -40452,7 +40454,7 @@
         <v>3</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F73" s="1">
         <v>1</v>
@@ -40469,8 +40471,8 @@
       <c r="D74" s="32">
         <v>3</v>
       </c>
-      <c r="E74" s="31" t="s">
-        <v>49</v>
+      <c r="E74" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F74" s="1">
         <v>1</v>
@@ -40821,7 +40823,7 @@
         <v>3</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F75" s="1">
         <v>1</v>
@@ -40838,8 +40840,8 @@
       <c r="D76" s="32">
         <v>3</v>
       </c>
-      <c r="E76" s="31" t="s">
-        <v>49</v>
+      <c r="E76" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F76" s="1">
         <v>1</v>
@@ -41190,7 +41192,7 @@
         <v>3</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F77" s="1">
         <v>1</v>
@@ -41207,8 +41209,8 @@
       <c r="D78" s="32">
         <v>3</v>
       </c>
-      <c r="E78" s="31" t="s">
-        <v>49</v>
+      <c r="E78" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F78" s="1">
         <v>1</v>
@@ -41559,7 +41561,7 @@
         <v>3</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F79" s="1">
         <v>1</v>
@@ -41576,8 +41578,8 @@
       <c r="D80" s="32">
         <v>3</v>
       </c>
-      <c r="E80" s="31" t="s">
-        <v>49</v>
+      <c r="E80" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F80" s="1">
         <v>1</v>
@@ -41928,7 +41930,7 @@
         <v>3</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F81" s="1">
         <v>1</v>
@@ -41945,8 +41947,8 @@
       <c r="D82" s="32">
         <v>3</v>
       </c>
-      <c r="E82" s="31" t="s">
-        <v>49</v>
+      <c r="E82" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F82" s="1">
         <v>1</v>
@@ -42297,7 +42299,7 @@
         <v>3</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F83" s="1">
         <v>1</v>
@@ -42314,8 +42316,8 @@
       <c r="D84" s="32">
         <v>3</v>
       </c>
-      <c r="E84" s="31" t="s">
-        <v>49</v>
+      <c r="E84" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="F84" s="1">
         <v>1</v>
@@ -42698,14 +42700,7 @@
       <c r="D108"/>
     </row>
   </sheetData>
-  <autoFilter ref="B27:I85" xr:uid="{49990737-28A7-44F3-B503-5D019EA27ABA}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Leonel - Nelson"/>
-        <filter val="Nelson"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B27:I85" xr:uid="{49990737-28A7-44F3-B503-5D019EA27ABA}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>